<commit_message>
add list add one leetcode
</commit_message>
<xml_diff>
--- a/LeetCode/python/facebook/facebook.xlsx
+++ b/LeetCode/python/facebook/facebook.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fang/Programs/Personal/coding/CodingTest/LeetCode/python/facebook/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\github\CodingTest\LeetCode\python\facebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6097A95F-C110-294A-9FF1-8377A93682CD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24" yWindow="456" windowWidth="28800" windowHeight="16620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$114</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="133">
   <si>
     <t>Design TinyURL</t>
   </si>
@@ -447,12 +446,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -465,7 +464,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -505,7 +504,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -782,20 +781,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
+      <selection pane="bottomLeft" activeCell="I102" sqref="I102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -817,7 +816,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="23">
+    <row r="2" spans="1:5" ht="22.8">
       <c r="A2" s="1">
         <v>534</v>
       </c>
@@ -831,7 +830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="23" hidden="1">
+    <row r="3" spans="1:5" ht="22.8" hidden="1">
       <c r="A3" s="1">
         <v>283</v>
       </c>
@@ -848,7 +847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="23" hidden="1">
+    <row r="4" spans="1:5" ht="22.8" hidden="1">
       <c r="A4" s="1">
         <v>301</v>
       </c>
@@ -862,7 +861,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="23" hidden="1">
+    <row r="5" spans="1:5" ht="22.8" hidden="1">
       <c r="A5" s="1">
         <v>273</v>
       </c>
@@ -879,7 +878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="23" hidden="1">
+    <row r="6" spans="1:5" ht="22.8" hidden="1">
       <c r="A6" s="1">
         <v>621</v>
       </c>
@@ -896,7 +895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="23" hidden="1">
+    <row r="7" spans="1:5" ht="22.8" hidden="1">
       <c r="A7" s="1">
         <v>67</v>
       </c>
@@ -913,7 +912,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="23" hidden="1">
+    <row r="8" spans="1:5" ht="22.8" hidden="1">
       <c r="A8" s="1">
         <v>689</v>
       </c>
@@ -927,7 +926,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="23">
+    <row r="9" spans="1:5" ht="22.8">
       <c r="A9" s="1">
         <v>325</v>
       </c>
@@ -944,7 +943,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="23">
+    <row r="10" spans="1:5" ht="22.8">
       <c r="A10" s="1">
         <v>253</v>
       </c>
@@ -961,7 +960,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="23" hidden="1">
+    <row r="11" spans="1:5" ht="22.8" hidden="1">
       <c r="A11" s="1">
         <v>17</v>
       </c>
@@ -978,7 +977,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="23" hidden="1">
+    <row r="12" spans="1:5" ht="22.8" hidden="1">
       <c r="A12" s="1">
         <v>91</v>
       </c>
@@ -995,7 +994,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="23">
+    <row r="13" spans="1:5" ht="22.8">
       <c r="A13" s="1">
         <v>311</v>
       </c>
@@ -1012,7 +1011,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="23" hidden="1">
+    <row r="14" spans="1:5" ht="22.8" hidden="1">
       <c r="A14" s="1">
         <v>297</v>
       </c>
@@ -1026,7 +1025,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="23">
+    <row r="15" spans="1:5" ht="22.8">
       <c r="A15" s="1">
         <v>314</v>
       </c>
@@ -1043,7 +1042,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="23" hidden="1">
+    <row r="16" spans="1:5" ht="22.8" hidden="1">
       <c r="A16" s="1">
         <v>158</v>
       </c>
@@ -1060,7 +1059,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="23" hidden="1">
+    <row r="17" spans="1:5" ht="22.8" hidden="1">
       <c r="A17" s="1">
         <v>10</v>
       </c>
@@ -1077,7 +1076,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="23" hidden="1">
+    <row r="18" spans="1:5" ht="22.8" hidden="1">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1094,7 +1093,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="23" hidden="1">
+    <row r="19" spans="1:5" ht="22.8" hidden="1">
       <c r="A19" s="1">
         <v>278</v>
       </c>
@@ -1111,7 +1110,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="23">
+    <row r="20" spans="1:5" ht="22.8">
       <c r="A20" s="1">
         <v>277</v>
       </c>
@@ -1128,7 +1127,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="23" hidden="1">
+    <row r="21" spans="1:5" ht="22.8" hidden="1">
       <c r="A21" s="1">
         <v>200</v>
       </c>
@@ -1145,7 +1144,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="23" hidden="1">
+    <row r="22" spans="1:5" ht="22.8" hidden="1">
       <c r="A22" s="1">
         <v>76</v>
       </c>
@@ -1159,7 +1158,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="23" hidden="1">
+    <row r="23" spans="1:5" ht="22.8" hidden="1">
       <c r="A23" s="1">
         <v>257</v>
       </c>
@@ -1173,7 +1172,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="23" hidden="1">
+    <row r="24" spans="1:5" ht="22.8" hidden="1">
       <c r="A24" s="1">
         <v>157</v>
       </c>
@@ -1190,7 +1189,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="23" hidden="1">
+    <row r="25" spans="1:5" ht="22.8" hidden="1">
       <c r="A25" s="1">
         <v>282</v>
       </c>
@@ -1204,7 +1203,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="23" hidden="1">
+    <row r="26" spans="1:5" ht="22.8" hidden="1">
       <c r="A26" s="1">
         <v>543</v>
       </c>
@@ -1218,7 +1217,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="23" hidden="1">
+    <row r="27" spans="1:5" ht="22.8" hidden="1">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -1235,7 +1234,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="23" hidden="1">
+    <row r="28" spans="1:5" ht="22.8" hidden="1">
       <c r="A28" s="1">
         <v>173</v>
       </c>
@@ -1252,7 +1251,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="23" hidden="1">
+    <row r="29" spans="1:5" ht="22.8" hidden="1">
       <c r="A29" s="1">
         <v>121</v>
       </c>
@@ -1269,7 +1268,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="23" hidden="1">
+    <row r="30" spans="1:5" ht="22.8" hidden="1">
       <c r="A30" s="1">
         <v>56</v>
       </c>
@@ -1286,7 +1285,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="23" hidden="1">
+    <row r="31" spans="1:5" ht="22.8" hidden="1">
       <c r="A31" s="1">
         <v>211</v>
       </c>
@@ -1303,7 +1302,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="23" hidden="1">
+    <row r="32" spans="1:5" ht="22.8" hidden="1">
       <c r="A32" s="1">
         <v>1</v>
       </c>
@@ -1320,7 +1319,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="23" hidden="1">
+    <row r="33" spans="1:5" ht="22.8" hidden="1">
       <c r="A33" s="1">
         <v>597</v>
       </c>
@@ -1337,7 +1336,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="23">
+    <row r="34" spans="1:5" ht="22.8">
       <c r="A34" s="1">
         <v>161</v>
       </c>
@@ -1354,7 +1353,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="23" hidden="1">
+    <row r="35" spans="1:5" ht="22.8" hidden="1">
       <c r="A35" s="1">
         <v>341</v>
       </c>
@@ -1371,7 +1370,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="23" hidden="1">
+    <row r="36" spans="1:5" ht="22.8" hidden="1">
       <c r="A36" s="1">
         <v>252</v>
       </c>
@@ -1388,7 +1387,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="23" hidden="1">
+    <row r="37" spans="1:5" ht="22.8" hidden="1">
       <c r="A37" s="1">
         <v>125</v>
       </c>
@@ -1402,7 +1401,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="23">
+    <row r="38" spans="1:5" ht="22.8">
       <c r="A38" s="1">
         <v>285</v>
       </c>
@@ -1419,7 +1418,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="23">
+    <row r="39" spans="1:5" ht="22.8">
       <c r="A39" s="1">
         <v>602</v>
       </c>
@@ -1436,7 +1435,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="23" hidden="1">
+    <row r="40" spans="1:5" ht="22.8" hidden="1">
       <c r="A40" s="1">
         <v>139</v>
       </c>
@@ -1453,7 +1452,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="23" hidden="1">
+    <row r="41" spans="1:5" ht="22.8" hidden="1">
       <c r="A41" s="1">
         <v>98</v>
       </c>
@@ -1470,7 +1469,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="23" hidden="1">
+    <row r="42" spans="1:5" ht="22.8" hidden="1">
       <c r="A42" s="1">
         <v>78</v>
       </c>
@@ -1487,7 +1486,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="23" hidden="1">
+    <row r="43" spans="1:5" ht="22.8" hidden="1">
       <c r="A43" s="1">
         <v>57</v>
       </c>
@@ -1501,7 +1500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="23" hidden="1">
+    <row r="44" spans="1:5" ht="22.8" hidden="1">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1518,7 +1517,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="23" hidden="1">
+    <row r="45" spans="1:5" ht="22.8" hidden="1">
       <c r="A45" s="1">
         <v>670</v>
       </c>
@@ -1535,7 +1534,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="23" hidden="1">
+    <row r="46" spans="1:5" ht="22.8" hidden="1">
       <c r="A46" s="1">
         <v>133</v>
       </c>
@@ -1552,7 +1551,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="23" hidden="1">
+    <row r="47" spans="1:5" ht="22.8" hidden="1">
       <c r="A47" s="1">
         <v>75</v>
       </c>
@@ -1569,7 +1568,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="23" hidden="1">
+    <row r="48" spans="1:5" ht="22.8" hidden="1">
       <c r="A48" s="1">
         <v>215</v>
       </c>
@@ -1586,7 +1585,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="23" hidden="1">
+    <row r="49" spans="1:5" ht="22.8" hidden="1">
       <c r="A49" s="1">
         <v>636</v>
       </c>
@@ -1603,7 +1602,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="23" hidden="1">
+    <row r="50" spans="1:5" ht="22.8" hidden="1">
       <c r="A50" s="1">
         <v>33</v>
       </c>
@@ -1620,7 +1619,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="23" hidden="1">
+    <row r="51" spans="1:5" ht="22.8" hidden="1">
       <c r="A51" s="1">
         <v>88</v>
       </c>
@@ -1637,7 +1636,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="23" hidden="1">
+    <row r="52" spans="1:5" ht="22.8" hidden="1">
       <c r="A52" s="1">
         <v>206</v>
       </c>
@@ -1654,7 +1653,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="23" hidden="1">
+    <row r="53" spans="1:5" ht="22.8" hidden="1">
       <c r="A53" s="1">
         <v>79</v>
       </c>
@@ -1671,7 +1670,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="23" hidden="1">
+    <row r="54" spans="1:5" ht="22.8" hidden="1">
       <c r="A54" s="1">
         <v>236</v>
       </c>
@@ -1688,7 +1687,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="23" hidden="1">
+    <row r="55" spans="1:5" ht="22.8" hidden="1">
       <c r="A55" s="1">
         <v>494</v>
       </c>
@@ -1705,7 +1704,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="23" hidden="1">
+    <row r="56" spans="1:5" ht="22.8" hidden="1">
       <c r="A56" s="1">
         <v>13</v>
       </c>
@@ -1722,7 +1721,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="23" hidden="1">
+    <row r="57" spans="1:5" ht="22.8" hidden="1">
       <c r="A57" s="1">
         <v>680</v>
       </c>
@@ -1736,7 +1735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="23" hidden="1">
+    <row r="58" spans="1:5" ht="22.8" hidden="1">
       <c r="A58" s="1">
         <v>238</v>
       </c>
@@ -1753,7 +1752,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="23" hidden="1">
+    <row r="59" spans="1:5" ht="22.8" hidden="1">
       <c r="A59" s="1">
         <v>477</v>
       </c>
@@ -1770,7 +1769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="23" hidden="1">
+    <row r="60" spans="1:5" ht="22.8" hidden="1">
       <c r="A60" s="1">
         <v>642</v>
       </c>
@@ -1787,7 +1786,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="23" hidden="1">
+    <row r="61" spans="1:5" ht="22.8" hidden="1">
       <c r="A61" s="1">
         <v>146</v>
       </c>
@@ -1804,7 +1803,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="23" hidden="1">
+    <row r="62" spans="1:5" ht="22.8" hidden="1">
       <c r="A62" s="1">
         <v>523</v>
       </c>
@@ -1821,7 +1820,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="23" hidden="1">
+    <row r="63" spans="1:5" ht="22.8" hidden="1">
       <c r="A63" s="1">
         <v>398</v>
       </c>
@@ -1838,7 +1837,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="23" hidden="1">
+    <row r="64" spans="1:5" ht="22.8" hidden="1">
       <c r="A64" s="1">
         <v>218</v>
       </c>
@@ -1855,7 +1854,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="23" hidden="1">
+    <row r="65" spans="1:5" ht="22.8" hidden="1">
       <c r="A65" s="1">
         <v>38</v>
       </c>
@@ -1869,7 +1868,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="23" hidden="1">
+    <row r="66" spans="1:5" ht="22.8" hidden="1">
       <c r="A66" s="1">
         <v>49</v>
       </c>
@@ -1886,7 +1885,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="23" hidden="1">
+    <row r="67" spans="1:5" ht="22.8" hidden="1">
       <c r="A67" s="1">
         <v>209</v>
       </c>
@@ -1903,7 +1902,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="23">
+    <row r="68" spans="1:5" ht="22.8">
       <c r="A68" s="1">
         <v>286</v>
       </c>
@@ -1920,7 +1919,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="23" hidden="1">
+    <row r="69" spans="1:5" ht="22.8" hidden="1">
       <c r="A69" s="1">
         <v>102</v>
       </c>
@@ -1937,7 +1936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="23" hidden="1">
+    <row r="70" spans="1:5" ht="22.8" hidden="1">
       <c r="A70" s="1">
         <v>208</v>
       </c>
@@ -1954,7 +1953,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="23" hidden="1">
+    <row r="71" spans="1:5" ht="22.8" hidden="1">
       <c r="A71" s="1">
         <v>554</v>
       </c>
@@ -1971,7 +1970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="23" hidden="1">
+    <row r="72" spans="1:5" ht="22.8" hidden="1">
       <c r="A72" s="1">
         <v>90</v>
       </c>
@@ -1988,7 +1987,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="23" hidden="1">
+    <row r="73" spans="1:5" ht="22.8" hidden="1">
       <c r="A73" s="1">
         <v>28</v>
       </c>
@@ -2005,7 +2004,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="23" hidden="1">
+    <row r="74" spans="1:5" ht="22.8" hidden="1">
       <c r="A74" s="1">
         <v>71</v>
       </c>
@@ -2022,7 +2021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="23" hidden="1">
+    <row r="75" spans="1:5" ht="22.8" hidden="1">
       <c r="A75" s="1">
         <v>128</v>
       </c>
@@ -2039,7 +2038,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="23" hidden="1">
+    <row r="76" spans="1:5" ht="22.8" hidden="1">
       <c r="A76" s="1">
         <v>20</v>
       </c>
@@ -2053,7 +2052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="23" hidden="1">
+    <row r="77" spans="1:5" ht="22.8" hidden="1">
       <c r="A77" s="1">
         <v>377</v>
       </c>
@@ -2070,7 +2069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="23" hidden="1">
+    <row r="78" spans="1:5" ht="22.8" hidden="1">
       <c r="A78" s="1">
         <v>127</v>
       </c>
@@ -2087,7 +2086,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="23" hidden="1">
+    <row r="79" spans="1:5" ht="22.8" hidden="1">
       <c r="A79" s="1">
         <v>44</v>
       </c>
@@ -2101,7 +2100,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="23" hidden="1">
+    <row r="80" spans="1:5" ht="22.8" hidden="1">
       <c r="A80" s="1">
         <v>334</v>
       </c>
@@ -2118,7 +2117,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="23" hidden="1">
+    <row r="81" spans="1:5" ht="22.8" hidden="1">
       <c r="A81" s="1">
         <v>269</v>
       </c>
@@ -2135,7 +2134,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="23" hidden="1">
+    <row r="82" spans="1:5" ht="22.8" hidden="1">
       <c r="A82" s="1">
         <v>639</v>
       </c>
@@ -2149,7 +2148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="23" hidden="1">
+    <row r="83" spans="1:5" ht="22.8" hidden="1">
       <c r="A83" s="1">
         <v>380</v>
       </c>
@@ -2166,7 +2165,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="23" hidden="1">
+    <row r="84" spans="1:5" ht="22.8" hidden="1">
       <c r="A84" s="1">
         <v>461</v>
       </c>
@@ -2180,7 +2179,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="23" hidden="1">
+    <row r="85" spans="1:5" ht="22.8" hidden="1">
       <c r="A85" s="1">
         <v>647</v>
       </c>
@@ -2197,7 +2196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="23" hidden="1">
+    <row r="86" spans="1:5" ht="22.8" hidden="1">
       <c r="A86" s="1">
         <v>235</v>
       </c>
@@ -2214,7 +2213,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="23" hidden="1">
+    <row r="87" spans="1:5" ht="22.8" hidden="1">
       <c r="A87" s="1">
         <v>50</v>
       </c>
@@ -2231,7 +2230,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="23" hidden="1">
+    <row r="88" spans="1:5" ht="22.8" hidden="1">
       <c r="A88" s="1">
         <v>117</v>
       </c>
@@ -2248,7 +2247,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="23" hidden="1">
+    <row r="89" spans="1:5" ht="22.8" hidden="1">
       <c r="A89" s="1">
         <v>85</v>
       </c>
@@ -2262,7 +2261,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="23" hidden="1">
+    <row r="90" spans="1:5" ht="22.8" hidden="1">
       <c r="A90" s="1">
         <v>69</v>
       </c>
@@ -2276,7 +2275,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="23" hidden="1">
+    <row r="91" spans="1:5" ht="22.8" hidden="1">
       <c r="A91" s="1">
         <v>68</v>
       </c>
@@ -2290,7 +2289,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="23" hidden="1">
+    <row r="92" spans="1:5" ht="22.8" hidden="1">
       <c r="A92" s="1">
         <v>210</v>
       </c>
@@ -2307,7 +2306,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="23" hidden="1">
+    <row r="93" spans="1:5" ht="22.8" hidden="1">
       <c r="A93" s="1">
         <v>26</v>
       </c>
@@ -2324,7 +2323,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="23" hidden="1">
+    <row r="94" spans="1:5" ht="22.8" hidden="1">
       <c r="A94" s="1">
         <v>221</v>
       </c>
@@ -2341,7 +2340,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="23">
+    <row r="95" spans="1:5" ht="22.8" hidden="1">
       <c r="A95" s="1">
         <v>274</v>
       </c>
@@ -2354,8 +2353,11 @@
       <c r="D95" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" ht="23" hidden="1">
+      <c r="E95" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="22.8" hidden="1">
       <c r="A96" s="1">
         <v>404</v>
       </c>
@@ -2369,7 +2371,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="23" hidden="1">
+    <row r="97" spans="1:5" ht="22.8" hidden="1">
       <c r="A97" s="1">
         <v>25</v>
       </c>
@@ -2383,7 +2385,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="23" hidden="1">
+    <row r="98" spans="1:5" ht="22.8" hidden="1">
       <c r="A98" s="1">
         <v>234</v>
       </c>
@@ -2397,7 +2399,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="23" hidden="1">
+    <row r="99" spans="1:5" ht="22.8" hidden="1">
       <c r="A99" s="1">
         <v>168</v>
       </c>
@@ -2411,7 +2413,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="23">
+    <row r="100" spans="1:5" ht="22.8">
       <c r="A100" s="1">
         <v>714</v>
       </c>
@@ -2425,7 +2427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:5" ht="23" hidden="1">
+    <row r="101" spans="1:5" ht="22.8" hidden="1">
       <c r="A101" s="1">
         <v>80</v>
       </c>
@@ -2442,7 +2444,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="23">
+    <row r="102" spans="1:5" ht="22.8">
       <c r="A102" s="1">
         <v>261</v>
       </c>
@@ -2459,7 +2461,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="23" hidden="1">
+    <row r="103" spans="1:5" ht="22.8" hidden="1">
       <c r="A103" s="1">
         <v>410</v>
       </c>
@@ -2473,7 +2475,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="23">
+    <row r="104" spans="1:5" ht="22.8">
       <c r="A104" s="1">
         <v>525</v>
       </c>
@@ -2487,7 +2489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:5" ht="23">
+    <row r="105" spans="1:5" ht="22.8">
       <c r="A105" s="1">
         <v>535</v>
       </c>
@@ -2501,7 +2503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="23" hidden="1">
+    <row r="106" spans="1:5" ht="22.8" hidden="1">
       <c r="A106" s="1">
         <v>265</v>
       </c>
@@ -2518,7 +2520,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="23">
+    <row r="107" spans="1:5" ht="22.8">
       <c r="A107" s="1">
         <v>721</v>
       </c>
@@ -2532,7 +2534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="23" hidden="1">
+    <row r="108" spans="1:5" ht="22.8" hidden="1">
       <c r="A108" s="1">
         <v>572</v>
       </c>
@@ -2546,7 +2548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="23">
+    <row r="109" spans="1:5" ht="22.8">
       <c r="A109" s="1">
         <v>578</v>
       </c>
@@ -2563,7 +2565,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="23" hidden="1">
+    <row r="110" spans="1:5" ht="22.8" hidden="1">
       <c r="A110" s="1">
         <v>637</v>
       </c>
@@ -2577,7 +2579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="23" hidden="1">
+    <row r="111" spans="1:5" ht="22.8" hidden="1">
       <c r="A111" s="1">
         <v>653</v>
       </c>
@@ -2591,7 +2593,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="23" hidden="1">
+    <row r="112" spans="1:5" ht="22.8" hidden="1">
       <c r="A112" s="1">
         <v>673</v>
       </c>
@@ -2608,7 +2610,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="23" hidden="1">
+    <row r="113" spans="1:5" ht="22.8" hidden="1">
       <c r="A113" s="1">
         <v>674</v>
       </c>
@@ -2622,7 +2624,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="23" hidden="1">
+    <row r="114" spans="1:5" ht="22.8" hidden="1">
       <c r="A114" s="1">
         <v>275</v>
       </c>
@@ -2640,7 +2642,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E114" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:E114">
     <filterColumn colId="3">
       <filters>
         <filter val="Medium"/>

</xml_diff>

<commit_message>
add 5 fb, finish fb medium
</commit_message>
<xml_diff>
--- a/LeetCode/python/facebook/facebook.xlsx
+++ b/LeetCode/python/facebook/facebook.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\github\CodingTest\LeetCode\python\facebook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fang/Programs/Personal/coding/CodingTest/LeetCode/python/facebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D7E6EC-C8AF-BF4D-8256-040F78685A37}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24" yWindow="456" windowWidth="28800" windowHeight="16620"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="133">
   <si>
     <t>Design TinyURL</t>
   </si>
@@ -446,12 +447,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -464,7 +465,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -504,7 +505,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -781,20 +782,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I102" sqref="I102"/>
+      <selection pane="bottomLeft" activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="60" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -816,7 +817,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="22.8">
+    <row r="2" spans="1:5" ht="23">
       <c r="A2" s="1">
         <v>534</v>
       </c>
@@ -830,7 +831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="22.8" hidden="1">
+    <row r="3" spans="1:5" ht="23" hidden="1">
       <c r="A3" s="1">
         <v>283</v>
       </c>
@@ -847,7 +848,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="22.8" hidden="1">
+    <row r="4" spans="1:5" ht="23" hidden="1">
       <c r="A4" s="1">
         <v>301</v>
       </c>
@@ -861,7 +862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="22.8" hidden="1">
+    <row r="5" spans="1:5" ht="23" hidden="1">
       <c r="A5" s="1">
         <v>273</v>
       </c>
@@ -878,7 +879,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="22.8" hidden="1">
+    <row r="6" spans="1:5" ht="23" hidden="1">
       <c r="A6" s="1">
         <v>621</v>
       </c>
@@ -895,7 +896,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="22.8" hidden="1">
+    <row r="7" spans="1:5" ht="23" hidden="1">
       <c r="A7" s="1">
         <v>67</v>
       </c>
@@ -912,7 +913,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="22.8" hidden="1">
+    <row r="8" spans="1:5" ht="23" hidden="1">
       <c r="A8" s="1">
         <v>689</v>
       </c>
@@ -926,7 +927,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="22.8">
+    <row r="9" spans="1:5" ht="23">
       <c r="A9" s="1">
         <v>325</v>
       </c>
@@ -943,7 +944,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="22.8">
+    <row r="10" spans="1:5" ht="23">
       <c r="A10" s="1">
         <v>253</v>
       </c>
@@ -960,7 +961,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="22.8" hidden="1">
+    <row r="11" spans="1:5" ht="23" hidden="1">
       <c r="A11" s="1">
         <v>17</v>
       </c>
@@ -977,7 +978,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="22.8" hidden="1">
+    <row r="12" spans="1:5" ht="23" hidden="1">
       <c r="A12" s="1">
         <v>91</v>
       </c>
@@ -994,7 +995,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="22.8">
+    <row r="13" spans="1:5" ht="23">
       <c r="A13" s="1">
         <v>311</v>
       </c>
@@ -1011,7 +1012,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="22.8" hidden="1">
+    <row r="14" spans="1:5" ht="23" hidden="1">
       <c r="A14" s="1">
         <v>297</v>
       </c>
@@ -1025,7 +1026,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="22.8">
+    <row r="15" spans="1:5" ht="23">
       <c r="A15" s="1">
         <v>314</v>
       </c>
@@ -1042,7 +1043,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="22.8" hidden="1">
+    <row r="16" spans="1:5" ht="23" hidden="1">
       <c r="A16" s="1">
         <v>158</v>
       </c>
@@ -1059,7 +1060,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="22.8" hidden="1">
+    <row r="17" spans="1:5" ht="23" hidden="1">
       <c r="A17" s="1">
         <v>10</v>
       </c>
@@ -1076,7 +1077,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="22.8" hidden="1">
+    <row r="18" spans="1:5" ht="23" hidden="1">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1093,7 +1094,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="22.8" hidden="1">
+    <row r="19" spans="1:5" ht="23" hidden="1">
       <c r="A19" s="1">
         <v>278</v>
       </c>
@@ -1110,7 +1111,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="22.8">
+    <row r="20" spans="1:5" ht="23">
       <c r="A20" s="1">
         <v>277</v>
       </c>
@@ -1127,7 +1128,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="22.8" hidden="1">
+    <row r="21" spans="1:5" ht="23" hidden="1">
       <c r="A21" s="1">
         <v>200</v>
       </c>
@@ -1144,7 +1145,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="22.8" hidden="1">
+    <row r="22" spans="1:5" ht="23" hidden="1">
       <c r="A22" s="1">
         <v>76</v>
       </c>
@@ -1158,7 +1159,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="22.8" hidden="1">
+    <row r="23" spans="1:5" ht="23" hidden="1">
       <c r="A23" s="1">
         <v>257</v>
       </c>
@@ -1172,7 +1173,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="22.8" hidden="1">
+    <row r="24" spans="1:5" ht="23" hidden="1">
       <c r="A24" s="1">
         <v>157</v>
       </c>
@@ -1189,7 +1190,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="22.8" hidden="1">
+    <row r="25" spans="1:5" ht="23" hidden="1">
       <c r="A25" s="1">
         <v>282</v>
       </c>
@@ -1203,7 +1204,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="22.8" hidden="1">
+    <row r="26" spans="1:5" ht="23" hidden="1">
       <c r="A26" s="1">
         <v>543</v>
       </c>
@@ -1217,7 +1218,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="22.8" hidden="1">
+    <row r="27" spans="1:5" ht="23" hidden="1">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -1234,7 +1235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="22.8" hidden="1">
+    <row r="28" spans="1:5" ht="23" hidden="1">
       <c r="A28" s="1">
         <v>173</v>
       </c>
@@ -1251,7 +1252,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="22.8" hidden="1">
+    <row r="29" spans="1:5" ht="23" hidden="1">
       <c r="A29" s="1">
         <v>121</v>
       </c>
@@ -1268,7 +1269,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="22.8" hidden="1">
+    <row r="30" spans="1:5" ht="23" hidden="1">
       <c r="A30" s="1">
         <v>56</v>
       </c>
@@ -1285,7 +1286,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="22.8" hidden="1">
+    <row r="31" spans="1:5" ht="23" hidden="1">
       <c r="A31" s="1">
         <v>211</v>
       </c>
@@ -1302,7 +1303,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="22.8" hidden="1">
+    <row r="32" spans="1:5" ht="23" hidden="1">
       <c r="A32" s="1">
         <v>1</v>
       </c>
@@ -1319,7 +1320,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="22.8" hidden="1">
+    <row r="33" spans="1:5" ht="23" hidden="1">
       <c r="A33" s="1">
         <v>597</v>
       </c>
@@ -1336,7 +1337,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="22.8">
+    <row r="34" spans="1:5" ht="23">
       <c r="A34" s="1">
         <v>161</v>
       </c>
@@ -1353,7 +1354,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="22.8" hidden="1">
+    <row r="35" spans="1:5" ht="23" hidden="1">
       <c r="A35" s="1">
         <v>341</v>
       </c>
@@ -1370,7 +1371,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="22.8" hidden="1">
+    <row r="36" spans="1:5" ht="23" hidden="1">
       <c r="A36" s="1">
         <v>252</v>
       </c>
@@ -1387,7 +1388,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="22.8" hidden="1">
+    <row r="37" spans="1:5" ht="23" hidden="1">
       <c r="A37" s="1">
         <v>125</v>
       </c>
@@ -1401,7 +1402,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="22.8">
+    <row r="38" spans="1:5" ht="23">
       <c r="A38" s="1">
         <v>285</v>
       </c>
@@ -1418,7 +1419,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="22.8">
+    <row r="39" spans="1:5" ht="23">
       <c r="A39" s="1">
         <v>602</v>
       </c>
@@ -1435,7 +1436,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="22.8" hidden="1">
+    <row r="40" spans="1:5" ht="23" hidden="1">
       <c r="A40" s="1">
         <v>139</v>
       </c>
@@ -1452,7 +1453,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="22.8" hidden="1">
+    <row r="41" spans="1:5" ht="23" hidden="1">
       <c r="A41" s="1">
         <v>98</v>
       </c>
@@ -1469,7 +1470,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="22.8" hidden="1">
+    <row r="42" spans="1:5" ht="23" hidden="1">
       <c r="A42" s="1">
         <v>78</v>
       </c>
@@ -1486,7 +1487,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="22.8" hidden="1">
+    <row r="43" spans="1:5" ht="23" hidden="1">
       <c r="A43" s="1">
         <v>57</v>
       </c>
@@ -1500,7 +1501,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="22.8" hidden="1">
+    <row r="44" spans="1:5" ht="23" hidden="1">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -1517,7 +1518,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="22.8" hidden="1">
+    <row r="45" spans="1:5" ht="23" hidden="1">
       <c r="A45" s="1">
         <v>670</v>
       </c>
@@ -1534,7 +1535,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="22.8" hidden="1">
+    <row r="46" spans="1:5" ht="23" hidden="1">
       <c r="A46" s="1">
         <v>133</v>
       </c>
@@ -1551,7 +1552,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="22.8" hidden="1">
+    <row r="47" spans="1:5" ht="23" hidden="1">
       <c r="A47" s="1">
         <v>75</v>
       </c>
@@ -1568,7 +1569,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="22.8" hidden="1">
+    <row r="48" spans="1:5" ht="23" hidden="1">
       <c r="A48" s="1">
         <v>215</v>
       </c>
@@ -1585,7 +1586,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="22.8" hidden="1">
+    <row r="49" spans="1:5" ht="23" hidden="1">
       <c r="A49" s="1">
         <v>636</v>
       </c>
@@ -1602,7 +1603,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="22.8" hidden="1">
+    <row r="50" spans="1:5" ht="23" hidden="1">
       <c r="A50" s="1">
         <v>33</v>
       </c>
@@ -1619,7 +1620,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="22.8" hidden="1">
+    <row r="51" spans="1:5" ht="23" hidden="1">
       <c r="A51" s="1">
         <v>88</v>
       </c>
@@ -1636,7 +1637,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="22.8" hidden="1">
+    <row r="52" spans="1:5" ht="23" hidden="1">
       <c r="A52" s="1">
         <v>206</v>
       </c>
@@ -1653,7 +1654,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="22.8" hidden="1">
+    <row r="53" spans="1:5" ht="23" hidden="1">
       <c r="A53" s="1">
         <v>79</v>
       </c>
@@ -1670,7 +1671,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="22.8" hidden="1">
+    <row r="54" spans="1:5" ht="23" hidden="1">
       <c r="A54" s="1">
         <v>236</v>
       </c>
@@ -1687,7 +1688,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="22.8" hidden="1">
+    <row r="55" spans="1:5" ht="23" hidden="1">
       <c r="A55" s="1">
         <v>494</v>
       </c>
@@ -1704,7 +1705,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="22.8" hidden="1">
+    <row r="56" spans="1:5" ht="23" hidden="1">
       <c r="A56" s="1">
         <v>13</v>
       </c>
@@ -1721,7 +1722,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="22.8" hidden="1">
+    <row r="57" spans="1:5" ht="23" hidden="1">
       <c r="A57" s="1">
         <v>680</v>
       </c>
@@ -1735,7 +1736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="22.8" hidden="1">
+    <row r="58" spans="1:5" ht="23" hidden="1">
       <c r="A58" s="1">
         <v>238</v>
       </c>
@@ -1752,7 +1753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="22.8" hidden="1">
+    <row r="59" spans="1:5" ht="23" hidden="1">
       <c r="A59" s="1">
         <v>477</v>
       </c>
@@ -1769,7 +1770,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="22.8" hidden="1">
+    <row r="60" spans="1:5" ht="23" hidden="1">
       <c r="A60" s="1">
         <v>642</v>
       </c>
@@ -1786,7 +1787,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="22.8" hidden="1">
+    <row r="61" spans="1:5" ht="23" hidden="1">
       <c r="A61" s="1">
         <v>146</v>
       </c>
@@ -1803,7 +1804,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="22.8" hidden="1">
+    <row r="62" spans="1:5" ht="23" hidden="1">
       <c r="A62" s="1">
         <v>523</v>
       </c>
@@ -1820,7 +1821,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="22.8" hidden="1">
+    <row r="63" spans="1:5" ht="23" hidden="1">
       <c r="A63" s="1">
         <v>398</v>
       </c>
@@ -1837,7 +1838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="22.8" hidden="1">
+    <row r="64" spans="1:5" ht="23" hidden="1">
       <c r="A64" s="1">
         <v>218</v>
       </c>
@@ -1854,7 +1855,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="22.8" hidden="1">
+    <row r="65" spans="1:5" ht="23" hidden="1">
       <c r="A65" s="1">
         <v>38</v>
       </c>
@@ -1868,7 +1869,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="22.8" hidden="1">
+    <row r="66" spans="1:5" ht="23" hidden="1">
       <c r="A66" s="1">
         <v>49</v>
       </c>
@@ -1885,7 +1886,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="22.8" hidden="1">
+    <row r="67" spans="1:5" ht="23" hidden="1">
       <c r="A67" s="1">
         <v>209</v>
       </c>
@@ -1902,7 +1903,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="22.8">
+    <row r="68" spans="1:5" ht="23">
       <c r="A68" s="1">
         <v>286</v>
       </c>
@@ -1919,7 +1920,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="22.8" hidden="1">
+    <row r="69" spans="1:5" ht="23" hidden="1">
       <c r="A69" s="1">
         <v>102</v>
       </c>
@@ -1936,7 +1937,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="22.8" hidden="1">
+    <row r="70" spans="1:5" ht="23" hidden="1">
       <c r="A70" s="1">
         <v>208</v>
       </c>
@@ -1953,7 +1954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="22.8" hidden="1">
+    <row r="71" spans="1:5" ht="23" hidden="1">
       <c r="A71" s="1">
         <v>554</v>
       </c>
@@ -1970,7 +1971,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="22.8" hidden="1">
+    <row r="72" spans="1:5" ht="23" hidden="1">
       <c r="A72" s="1">
         <v>90</v>
       </c>
@@ -1987,7 +1988,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="22.8" hidden="1">
+    <row r="73" spans="1:5" ht="23" hidden="1">
       <c r="A73" s="1">
         <v>28</v>
       </c>
@@ -2004,7 +2005,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="22.8" hidden="1">
+    <row r="74" spans="1:5" ht="23" hidden="1">
       <c r="A74" s="1">
         <v>71</v>
       </c>
@@ -2021,7 +2022,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="22.8" hidden="1">
+    <row r="75" spans="1:5" ht="23" hidden="1">
       <c r="A75" s="1">
         <v>128</v>
       </c>
@@ -2038,7 +2039,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="22.8" hidden="1">
+    <row r="76" spans="1:5" ht="23" hidden="1">
       <c r="A76" s="1">
         <v>20</v>
       </c>
@@ -2052,7 +2053,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="22.8" hidden="1">
+    <row r="77" spans="1:5" ht="23" hidden="1">
       <c r="A77" s="1">
         <v>377</v>
       </c>
@@ -2069,7 +2070,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="22.8" hidden="1">
+    <row r="78" spans="1:5" ht="23" hidden="1">
       <c r="A78" s="1">
         <v>127</v>
       </c>
@@ -2086,7 +2087,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="22.8" hidden="1">
+    <row r="79" spans="1:5" ht="23" hidden="1">
       <c r="A79" s="1">
         <v>44</v>
       </c>
@@ -2100,7 +2101,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="22.8" hidden="1">
+    <row r="80" spans="1:5" ht="23" hidden="1">
       <c r="A80" s="1">
         <v>334</v>
       </c>
@@ -2117,7 +2118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="22.8" hidden="1">
+    <row r="81" spans="1:5" ht="23" hidden="1">
       <c r="A81" s="1">
         <v>269</v>
       </c>
@@ -2134,7 +2135,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="22.8" hidden="1">
+    <row r="82" spans="1:5" ht="23" hidden="1">
       <c r="A82" s="1">
         <v>639</v>
       </c>
@@ -2148,7 +2149,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="22.8" hidden="1">
+    <row r="83" spans="1:5" ht="23" hidden="1">
       <c r="A83" s="1">
         <v>380</v>
       </c>
@@ -2165,7 +2166,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="22.8" hidden="1">
+    <row r="84" spans="1:5" ht="23" hidden="1">
       <c r="A84" s="1">
         <v>461</v>
       </c>
@@ -2179,7 +2180,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="22.8" hidden="1">
+    <row r="85" spans="1:5" ht="23" hidden="1">
       <c r="A85" s="1">
         <v>647</v>
       </c>
@@ -2196,7 +2197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="22.8" hidden="1">
+    <row r="86" spans="1:5" ht="23" hidden="1">
       <c r="A86" s="1">
         <v>235</v>
       </c>
@@ -2213,7 +2214,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="22.8" hidden="1">
+    <row r="87" spans="1:5" ht="23" hidden="1">
       <c r="A87" s="1">
         <v>50</v>
       </c>
@@ -2230,7 +2231,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="22.8" hidden="1">
+    <row r="88" spans="1:5" ht="23" hidden="1">
       <c r="A88" s="1">
         <v>117</v>
       </c>
@@ -2247,7 +2248,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="22.8" hidden="1">
+    <row r="89" spans="1:5" ht="23" hidden="1">
       <c r="A89" s="1">
         <v>85</v>
       </c>
@@ -2261,7 +2262,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="22.8" hidden="1">
+    <row r="90" spans="1:5" ht="23" hidden="1">
       <c r="A90" s="1">
         <v>69</v>
       </c>
@@ -2275,7 +2276,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="22.8" hidden="1">
+    <row r="91" spans="1:5" ht="23" hidden="1">
       <c r="A91" s="1">
         <v>68</v>
       </c>
@@ -2289,7 +2290,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="22.8" hidden="1">
+    <row r="92" spans="1:5" ht="23" hidden="1">
       <c r="A92" s="1">
         <v>210</v>
       </c>
@@ -2306,7 +2307,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="22.8" hidden="1">
+    <row r="93" spans="1:5" ht="23" hidden="1">
       <c r="A93" s="1">
         <v>26</v>
       </c>
@@ -2323,7 +2324,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="22.8" hidden="1">
+    <row r="94" spans="1:5" ht="23" hidden="1">
       <c r="A94" s="1">
         <v>221</v>
       </c>
@@ -2340,7 +2341,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="22.8" hidden="1">
+    <row r="95" spans="1:5" ht="23" hidden="1">
       <c r="A95" s="1">
         <v>274</v>
       </c>
@@ -2357,7 +2358,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="22.8" hidden="1">
+    <row r="96" spans="1:5" ht="23" hidden="1">
       <c r="A96" s="1">
         <v>404</v>
       </c>
@@ -2371,7 +2372,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="22.8" hidden="1">
+    <row r="97" spans="1:5" ht="23" hidden="1">
       <c r="A97" s="1">
         <v>25</v>
       </c>
@@ -2385,7 +2386,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="22.8" hidden="1">
+    <row r="98" spans="1:5" ht="23" hidden="1">
       <c r="A98" s="1">
         <v>234</v>
       </c>
@@ -2399,7 +2400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="22.8" hidden="1">
+    <row r="99" spans="1:5" ht="23" hidden="1">
       <c r="A99" s="1">
         <v>168</v>
       </c>
@@ -2413,7 +2414,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="22.8">
+    <row r="100" spans="1:5" ht="23" hidden="1">
       <c r="A100" s="1">
         <v>714</v>
       </c>
@@ -2426,8 +2427,11 @@
       <c r="D100" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" ht="22.8" hidden="1">
+      <c r="E100" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="23" hidden="1">
       <c r="A101" s="1">
         <v>80</v>
       </c>
@@ -2444,7 +2448,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="22.8">
+    <row r="102" spans="1:5" ht="23">
       <c r="A102" s="1">
         <v>261</v>
       </c>
@@ -2461,7 +2465,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="22.8" hidden="1">
+    <row r="103" spans="1:5" ht="23" hidden="1">
       <c r="A103" s="1">
         <v>410</v>
       </c>
@@ -2475,7 +2479,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="22.8">
+    <row r="104" spans="1:5" ht="23" hidden="1">
       <c r="A104" s="1">
         <v>525</v>
       </c>
@@ -2488,8 +2492,11 @@
       <c r="D104" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" ht="22.8">
+      <c r="E104" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="23" hidden="1">
       <c r="A105" s="1">
         <v>535</v>
       </c>
@@ -2502,8 +2509,11 @@
       <c r="D105" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" ht="22.8" hidden="1">
+      <c r="E105" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="23" hidden="1">
       <c r="A106" s="1">
         <v>265</v>
       </c>
@@ -2520,7 +2530,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="22.8">
+    <row r="107" spans="1:5" ht="23" hidden="1">
       <c r="A107" s="1">
         <v>721</v>
       </c>
@@ -2533,8 +2543,11 @@
       <c r="D107" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" ht="22.8" hidden="1">
+      <c r="E107" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="23" hidden="1">
       <c r="A108" s="1">
         <v>572</v>
       </c>
@@ -2548,7 +2561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="22.8">
+    <row r="109" spans="1:5" ht="23">
       <c r="A109" s="1">
         <v>578</v>
       </c>
@@ -2565,7 +2578,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="22.8" hidden="1">
+    <row r="110" spans="1:5" ht="23" hidden="1">
       <c r="A110" s="1">
         <v>637</v>
       </c>
@@ -2579,7 +2592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="22.8" hidden="1">
+    <row r="111" spans="1:5" ht="23" hidden="1">
       <c r="A111" s="1">
         <v>653</v>
       </c>
@@ -2593,7 +2606,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="22.8" hidden="1">
+    <row r="112" spans="1:5" ht="23" hidden="1">
       <c r="A112" s="1">
         <v>673</v>
       </c>
@@ -2610,7 +2623,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="22.8" hidden="1">
+    <row r="113" spans="1:5" ht="23" hidden="1">
       <c r="A113" s="1">
         <v>674</v>
       </c>
@@ -2624,7 +2637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="22.8" hidden="1">
+    <row r="114" spans="1:5" ht="23" hidden="1">
       <c r="A114" s="1">
         <v>275</v>
       </c>
@@ -2642,7 +2655,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E114">
+  <autoFilter ref="A1:E114" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="3">
       <filters>
         <filter val="Medium"/>

</xml_diff>